<commit_message>
Yet more PCA data analysis. It seems that both 'mfcc' and 'tonnetz' datasets have most bang for buck. Hence created two excel sheets for extracting PCA data for 'mfcc' and 'tonnetz'
This can be reproduced by running create_pca_datasets.py
</commit_message>
<xml_diff>
--- a/fma/pca_analysis_output.xlsx
+++ b/fma/pca_analysis_output.xlsx
@@ -18,15 +18,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">analysis!$A$1:$E$78</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId3"/>
+    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="14" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="31">
   <si>
     <t>Column Labels</t>
   </si>
@@ -105,6 +106,21 @@
   <si>
     <t>Average of % REDUCTION</t>
   </si>
+  <si>
+    <t>Sum of PCA</t>
+  </si>
+  <si>
+    <t>Total number of PCA columns</t>
+  </si>
+  <si>
+    <t>% REDUCTION / PCA</t>
+  </si>
+  <si>
+    <t>Sum of % REDUCTION / PCA</t>
+  </si>
+  <si>
+    <t>Total of % REDUCTION / PCA</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -186,11 +202,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -203,11 +234,787 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="80">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="medium">
@@ -317,6 +1124,59 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Ksheerasagar Akella" refreshedDate="42977.089148842591" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="77">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:F78" sheet="analysis"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="FEATURE" numFmtId="0">
+      <sharedItems count="11">
+        <s v="chroma_stft"/>
+        <s v="chroma_cqt"/>
+        <s v="chroma_cens"/>
+        <s v="tonnetz"/>
+        <s v="mfcc"/>
+        <s v="rmse"/>
+        <s v="zcr"/>
+        <s v="spectral_centroid"/>
+        <s v="spectral_bandwidth"/>
+        <s v="spectral_contrast"/>
+        <s v="spectral_rolloff"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ATTRIBUTE" numFmtId="0">
+      <sharedItems count="7">
+        <s v="kurtosis"/>
+        <s v="mean"/>
+        <s v="min"/>
+        <s v="max"/>
+        <s v="skew"/>
+        <s v="median"/>
+        <s v="std"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="ORIGINAL" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="20"/>
+    </cacheField>
+    <cacheField name="PCA" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12"/>
+    </cacheField>
+    <cacheField name="% REDUCTION" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.9"/>
+    </cacheField>
+    <cacheField name="% REDUCTION / PCA" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.45"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="77">
   <r>
@@ -861,8 +1721,1014 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="77">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="12"/>
+    <n v="4"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.16666666666666666"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="12"/>
+    <n v="2"/>
+    <n v="0.83333333333333337"/>
+    <n v="0.41666666666666669"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="12"/>
+    <n v="6"/>
+    <n v="0.5"/>
+    <n v="8.3333333333333329E-2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="12"/>
+    <n v="9"/>
+    <n v="0.25"/>
+    <n v="2.7777777777777776E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="12"/>
+    <n v="2"/>
+    <n v="0.83333333333333337"/>
+    <n v="0.41666666666666669"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="12"/>
+    <n v="6"/>
+    <n v="0.5"/>
+    <n v="8.3333333333333329E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="12"/>
+    <n v="5"/>
+    <n v="0.58333333333333337"/>
+    <n v="0.11666666666666667"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="12"/>
+    <n v="6"/>
+    <n v="0.5"/>
+    <n v="8.3333333333333329E-2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="12"/>
+    <n v="9"/>
+    <n v="0.25"/>
+    <n v="2.7777777777777776E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="12"/>
+    <n v="6"/>
+    <n v="0.5"/>
+    <n v="8.3333333333333329E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="12"/>
+    <n v="9"/>
+    <n v="0.25"/>
+    <n v="2.7777777777777776E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="12"/>
+    <n v="9"/>
+    <n v="0.25"/>
+    <n v="2.7777777777777776E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="12"/>
+    <n v="7"/>
+    <n v="0.41666666666666669"/>
+    <n v="5.9523809523809527E-2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="12"/>
+    <n v="8"/>
+    <n v="0.33333333333333331"/>
+    <n v="4.1666666666666664E-2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="0.5"/>
+    <n v="0.16666666666666666"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="2"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.33333333333333331"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="0.5"/>
+    <n v="0.16666666666666666"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="0.5"/>
+    <n v="0.16666666666666666"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="0.16666666666666671"/>
+    <n v="3.333333333333334E-2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="6"/>
+    <n v="2"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.33333333333333331"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="6"/>
+    <n v="2"/>
+    <n v="0.66666666666666663"/>
+    <n v="0.33333333333333331"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="20"/>
+    <n v="2"/>
+    <n v="0.9"/>
+    <n v="0.45"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="20"/>
+    <n v="3"/>
+    <n v="0.85"/>
+    <n v="0.28333333333333333"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="20"/>
+    <n v="7"/>
+    <n v="0.65"/>
+    <n v="9.285714285714286E-2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="20"/>
+    <n v="5"/>
+    <n v="0.75"/>
+    <n v="0.15"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="20"/>
+    <n v="12"/>
+    <n v="0.4"/>
+    <n v="3.3333333333333333E-2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <n v="20"/>
+    <n v="3"/>
+    <n v="0.85"/>
+    <n v="0.28333333333333333"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="6"/>
+    <n v="20"/>
+    <n v="3"/>
+    <n v="0.85"/>
+    <n v="0.28333333333333333"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="6"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="6"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="0"/>
+    <n v="7"/>
+    <n v="3"/>
+    <n v="0.5714285714285714"/>
+    <n v="0.19047619047619047"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="7"/>
+    <n v="4"/>
+    <n v="0.42857142857142849"/>
+    <n v="0.10714285714285712"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="7"/>
+    <n v="4"/>
+    <n v="0.42857142857142849"/>
+    <n v="0.10714285714285712"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="0.2857142857142857"/>
+    <n v="5.7142857142857141E-2"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="4"/>
+    <n v="7"/>
+    <n v="4"/>
+    <n v="0.42857142857142849"/>
+    <n v="0.10714285714285712"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="5"/>
+    <n v="7"/>
+    <n v="4"/>
+    <n v="0.42857142857142849"/>
+    <n v="0.10714285714285712"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="6"/>
+    <n v="7"/>
+    <n v="4"/>
+    <n v="0.42857142857142849"/>
+    <n v="0.10714285714285712"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="2"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="4"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="5"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="6"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average of % REDUCTION" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total of % REDUCTION / PCA" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A39:I52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of % REDUCTION / PCA" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="10">
+    <format dxfId="38">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="40">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="41">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="42">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="43">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total number of PCA columns" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A21:I34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of PCA" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="72">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="73">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="74">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="75">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average of % REDUCTION" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:I16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -971,7 +2837,7 @@
     <dataField name="Average of % REDUCTION" fld="4" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="3">
+    <format dxfId="79">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -980,7 +2846,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -989,7 +2855,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="77">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -998,7 +2864,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -1280,18 +3146,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I16"/>
+  <dimension ref="A3:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1677,6 +3543,776 @@
       </c>
       <c r="I16" s="3">
         <v>0.2792207792207792</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="3">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3">
+        <v>6</v>
+      </c>
+      <c r="E23" s="3">
+        <v>7</v>
+      </c>
+      <c r="F23" s="3">
+        <v>7</v>
+      </c>
+      <c r="G23" s="3">
+        <v>9</v>
+      </c>
+      <c r="H23" s="3">
+        <v>8</v>
+      </c>
+      <c r="I23" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3">
+        <v>6</v>
+      </c>
+      <c r="F24" s="3">
+        <v>5</v>
+      </c>
+      <c r="G24" s="3">
+        <v>7</v>
+      </c>
+      <c r="H24" s="3">
+        <v>9</v>
+      </c>
+      <c r="I24" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="3">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3">
+        <v>6</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>7</v>
+      </c>
+      <c r="H25" s="3">
+        <v>9</v>
+      </c>
+      <c r="I25" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3">
+        <v>7</v>
+      </c>
+      <c r="G26" s="3">
+        <v>12</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
+      <c r="I26" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4</v>
+      </c>
+      <c r="F30" s="3">
+        <v>4</v>
+      </c>
+      <c r="G30" s="3">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3">
+        <v>4</v>
+      </c>
+      <c r="I30" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="3">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3</v>
+      </c>
+      <c r="D32" s="3">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2</v>
+      </c>
+      <c r="F32" s="3">
+        <v>3</v>
+      </c>
+      <c r="G32" s="3">
+        <v>5</v>
+      </c>
+      <c r="H32" s="3">
+        <v>2</v>
+      </c>
+      <c r="I32" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="3">
+        <v>26</v>
+      </c>
+      <c r="C34" s="3">
+        <v>41</v>
+      </c>
+      <c r="D34" s="3">
+        <v>33</v>
+      </c>
+      <c r="E34" s="3">
+        <v>33</v>
+      </c>
+      <c r="F34" s="3">
+        <v>33</v>
+      </c>
+      <c r="G34" s="3">
+        <v>49</v>
+      </c>
+      <c r="H34" s="3">
+        <v>40</v>
+      </c>
+      <c r="I34" s="3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E41" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="F41" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="G41" s="3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H41" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0.35912698412698418</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C42" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="D42" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E42" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.11666666666666667</v>
+      </c>
+      <c r="G42" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0.84682539682539693</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C43" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="D43" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="E43" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G43" s="3">
+        <v>5.9523809523809527E-2</v>
+      </c>
+      <c r="H43" s="3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0.87301587301587302</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="C44" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="E44" s="6">
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="F44" s="6">
+        <v>9.285714285714286E-2</v>
+      </c>
+      <c r="G44" s="6">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H44" s="6">
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="I44" s="7">
+        <v>1.5761904761904764</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="C48" s="3">
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.10714285714285712</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.10714285714285712</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.10714285714285712</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0.10714285714285712</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0.10714285714285712</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0.7833333333333331</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D50" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E50" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F50" s="6">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G50" s="6">
+        <v>3.333333333333334E-2</v>
+      </c>
+      <c r="H50" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I50" s="7">
+        <v>1.5333333333333334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1.4500000000000002</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0.52063492063492067</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.95952380952380945</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0.32063492063492061</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0.821031746031746</v>
+      </c>
+      <c r="I52" s="3">
+        <v>5.9718253968253965</v>
       </c>
     </row>
   </sheetData>
@@ -1686,11 +4322,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,9 +4335,10 @@
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -1718,8 +4354,11 @@
       <c r="E1" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1735,8 +4374,12 @@
       <c r="E2">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>E2/D2</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1752,8 +4395,12 @@
       <c r="E3">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">E3/D3</f>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1769,8 +4416,12 @@
       <c r="E4">
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1786,8 +4437,12 @@
       <c r="E5">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1803,8 +4458,12 @@
       <c r="E6">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1820,8 +4479,12 @@
       <c r="E7">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1837,8 +4500,12 @@
       <c r="E8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1854,8 +4521,12 @@
       <c r="E9">
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1871,8 +4542,12 @@
       <c r="E10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1888,8 +4563,12 @@
       <c r="E11">
         <v>0.58333333333333337</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.11666666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1905,8 +4584,12 @@
       <c r="E12">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1922,8 +4605,12 @@
       <c r="E13">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1939,8 +4626,12 @@
       <c r="E14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1956,8 +4647,12 @@
       <c r="E15">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1973,8 +4668,12 @@
       <c r="E16">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1990,8 +4689,12 @@
       <c r="E17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2007,8 +4710,12 @@
       <c r="E18">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2024,8 +4731,12 @@
       <c r="E19">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -2041,8 +4752,12 @@
       <c r="E20">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2058,8 +4773,12 @@
       <c r="E21">
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>5.9523809523809527E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2075,8 +4794,12 @@
       <c r="E22">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2092,8 +4815,12 @@
       <c r="E23">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2109,8 +4836,12 @@
       <c r="E24">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2126,8 +4857,12 @@
       <c r="E25">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2143,8 +4878,12 @@
       <c r="E26">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -2160,8 +4899,12 @@
       <c r="E27">
         <v>0.16666666666666671</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>3.333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -2177,8 +4920,12 @@
       <c r="E28">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -2194,8 +4941,12 @@
       <c r="E29">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2211,8 +4962,12 @@
       <c r="E30">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2228,8 +4983,12 @@
       <c r="E31">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -2245,8 +5004,12 @@
       <c r="E32">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>9.285714285714286E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -2262,8 +5025,12 @@
       <c r="E33">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -2279,8 +5046,12 @@
       <c r="E34">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2296,8 +5067,12 @@
       <c r="E35">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2313,8 +5088,12 @@
       <c r="E36">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -2330,8 +5109,12 @@
       <c r="E37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -2347,8 +5130,12 @@
       <c r="E38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2364,8 +5151,12 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2381,8 +5172,12 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -2398,8 +5193,12 @@
       <c r="E41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>13</v>
       </c>
@@ -2415,8 +5214,12 @@
       <c r="E42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2432,8 +5235,12 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2449,8 +5256,12 @@
       <c r="E44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -2466,8 +5277,12 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -2483,8 +5298,12 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -2500,8 +5319,12 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -2517,8 +5340,12 @@
       <c r="E48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -2534,8 +5361,12 @@
       <c r="E49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -2551,8 +5382,12 @@
       <c r="E50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -2568,8 +5403,12 @@
       <c r="E51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -2585,8 +5424,12 @@
       <c r="E52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2602,8 +5445,12 @@
       <c r="E53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
@@ -2619,8 +5466,12 @@
       <c r="E54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>15</v>
       </c>
@@ -2636,8 +5487,12 @@
       <c r="E55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -2653,8 +5508,12 @@
       <c r="E56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -2670,8 +5529,12 @@
       <c r="E57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -2687,8 +5550,12 @@
       <c r="E58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -2704,8 +5571,12 @@
       <c r="E59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -2721,8 +5592,12 @@
       <c r="E60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -2738,8 +5613,12 @@
       <c r="E61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -2755,8 +5634,12 @@
       <c r="E62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -2772,8 +5655,12 @@
       <c r="E63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -2789,8 +5676,12 @@
       <c r="E64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -2806,8 +5697,12 @@
       <c r="E65">
         <v>0.5714285714285714</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>0.19047619047619047</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2823,8 +5718,12 @@
       <c r="E66">
         <v>0.42857142857142849</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>0.10714285714285712</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -2840,8 +5739,12 @@
       <c r="E67">
         <v>0.42857142857142849</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" ref="F67:F78" si="1">E67/D67</f>
+        <v>0.10714285714285712</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2857,8 +5760,12 @@
       <c r="E68">
         <v>0.2857142857142857</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2874,8 +5781,12 @@
       <c r="E69">
         <v>0.42857142857142849</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>0.10714285714285712</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2891,8 +5802,12 @@
       <c r="E70">
         <v>0.42857142857142849</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>0.10714285714285712</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -2908,8 +5823,12 @@
       <c r="E71">
         <v>0.42857142857142849</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>0.10714285714285712</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -2925,8 +5844,12 @@
       <c r="E72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -2942,8 +5865,12 @@
       <c r="E73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -2959,8 +5886,12 @@
       <c r="E74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>17</v>
       </c>
@@ -2976,8 +5907,12 @@
       <c r="E75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -2993,8 +5928,12 @@
       <c r="E76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -3010,8 +5949,12 @@
       <c r="E77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -3027,15 +5970,12 @@
       <c r="E78">
         <v>0</v>
       </c>
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E78">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="mfcc"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Color coded features with single attribute columns in gray to highlight that the PCA analysis tells us nothing about the effectiveness of using these features
</commit_message>
<xml_diff>
--- a/fma/pca_analysis_output.xlsx
+++ b/fma/pca_analysis_output.xlsx
@@ -20,8 +20,8 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
-    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="15" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -143,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -238,618 +244,96 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
     </dxf>
@@ -866,28 +350,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -984,36 +446,50 @@
       </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -2343,7 +1819,395 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total of % REDUCTION / PCA" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total number of PCA columns" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A21:I34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of PCA" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="6">
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average of % REDUCTION" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:I16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of % REDUCTION" fld="4" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="10">
+    <format dxfId="21">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="3">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="3">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total of % REDUCTION / PCA" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A39:I52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -2452,8 +2316,8 @@
   <dataFields count="1">
     <dataField name="Sum of % REDUCTION / PCA" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="10">
-    <format dxfId="38">
+  <formats count="16">
+    <format dxfId="31">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2462,7 +2326,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2471,7 +2335,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="29">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2480,7 +2344,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2489,7 +2353,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="27">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2498,7 +2362,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2507,7 +2371,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="25">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2516,7 +2380,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2525,7 +2389,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2534,7 +2398,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2543,332 +2407,60 @@
         </references>
       </pivotArea>
     </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Total number of PCA columns" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A21:I34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="12">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="8">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="12">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of PCA" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="6">
-    <format dxfId="72">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
+          <reference field="0" count="3">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
+          <reference field="0" count="3">
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
-            <x v="3"/>
+            <x v="8"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
-            <x v="3"/>
+            <x v="8"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
-            <x v="3"/>
+            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average of % REDUCTION" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:I16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="12">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="8">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="12">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of % REDUCTION" fld="4" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="79">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="78">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="77">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="76">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1">
-            <x v="3"/>
+            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
@@ -3148,8 +2740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,89 +2906,89 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="B9" s="11">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
+      <c r="B10" s="11">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="B11" s="11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
         <v>0</v>
       </c>
     </row>
@@ -3430,31 +3022,31 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
+      <c r="B13" s="11">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
         <v>0</v>
       </c>
     </row>
@@ -3488,31 +3080,31 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4084,89 +3676,89 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="3">
-        <v>0</v>
-      </c>
-      <c r="C45" s="3">
-        <v>0</v>
-      </c>
-      <c r="D45" s="3">
-        <v>0</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0</v>
-      </c>
-      <c r="F45" s="3">
-        <v>0</v>
-      </c>
-      <c r="G45" s="3">
-        <v>0</v>
-      </c>
-      <c r="H45" s="3">
-        <v>0</v>
-      </c>
-      <c r="I45" s="3">
+      <c r="B45" s="11">
+        <v>0</v>
+      </c>
+      <c r="C45" s="11">
+        <v>0</v>
+      </c>
+      <c r="D45" s="11">
+        <v>0</v>
+      </c>
+      <c r="E45" s="11">
+        <v>0</v>
+      </c>
+      <c r="F45" s="11">
+        <v>0</v>
+      </c>
+      <c r="G45" s="11">
+        <v>0</v>
+      </c>
+      <c r="H45" s="11">
+        <v>0</v>
+      </c>
+      <c r="I45" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="3">
-        <v>0</v>
-      </c>
-      <c r="C46" s="3">
-        <v>0</v>
-      </c>
-      <c r="D46" s="3">
-        <v>0</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0</v>
-      </c>
-      <c r="G46" s="3">
-        <v>0</v>
-      </c>
-      <c r="H46" s="3">
-        <v>0</v>
-      </c>
-      <c r="I46" s="3">
+      <c r="B46" s="11">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11">
+        <v>0</v>
+      </c>
+      <c r="D46" s="11">
+        <v>0</v>
+      </c>
+      <c r="E46" s="11">
+        <v>0</v>
+      </c>
+      <c r="F46" s="11">
+        <v>0</v>
+      </c>
+      <c r="G46" s="11">
+        <v>0</v>
+      </c>
+      <c r="H46" s="11">
+        <v>0</v>
+      </c>
+      <c r="I46" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="3">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3">
-        <v>0</v>
-      </c>
-      <c r="D47" s="3">
-        <v>0</v>
-      </c>
-      <c r="E47" s="3">
-        <v>0</v>
-      </c>
-      <c r="F47" s="3">
-        <v>0</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0</v>
-      </c>
-      <c r="H47" s="3">
-        <v>0</v>
-      </c>
-      <c r="I47" s="3">
+      <c r="B47" s="11">
+        <v>0</v>
+      </c>
+      <c r="C47" s="11">
+        <v>0</v>
+      </c>
+      <c r="D47" s="11">
+        <v>0</v>
+      </c>
+      <c r="E47" s="11">
+        <v>0</v>
+      </c>
+      <c r="F47" s="11">
+        <v>0</v>
+      </c>
+      <c r="G47" s="11">
+        <v>0</v>
+      </c>
+      <c r="H47" s="11">
+        <v>0</v>
+      </c>
+      <c r="I47" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4200,31 +3792,31 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="3">
-        <v>0</v>
-      </c>
-      <c r="C49" s="3">
-        <v>0</v>
-      </c>
-      <c r="D49" s="3">
-        <v>0</v>
-      </c>
-      <c r="E49" s="3">
-        <v>0</v>
-      </c>
-      <c r="F49" s="3">
-        <v>0</v>
-      </c>
-      <c r="G49" s="3">
-        <v>0</v>
-      </c>
-      <c r="H49" s="3">
-        <v>0</v>
-      </c>
-      <c r="I49" s="3">
+      <c r="B49" s="11">
+        <v>0</v>
+      </c>
+      <c r="C49" s="11">
+        <v>0</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0</v>
+      </c>
+      <c r="E49" s="11">
+        <v>0</v>
+      </c>
+      <c r="F49" s="11">
+        <v>0</v>
+      </c>
+      <c r="G49" s="11">
+        <v>0</v>
+      </c>
+      <c r="H49" s="11">
+        <v>0</v>
+      </c>
+      <c r="I49" s="11">
         <v>0</v>
       </c>
     </row>
@@ -4258,31 +3850,31 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B51" s="3">
-        <v>0</v>
-      </c>
-      <c r="C51" s="3">
-        <v>0</v>
-      </c>
-      <c r="D51" s="3">
-        <v>0</v>
-      </c>
-      <c r="E51" s="3">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3">
-        <v>0</v>
-      </c>
-      <c r="G51" s="3">
-        <v>0</v>
-      </c>
-      <c r="H51" s="3">
-        <v>0</v>
-      </c>
-      <c r="I51" s="3">
+      <c r="B51" s="11">
+        <v>0</v>
+      </c>
+      <c r="C51" s="11">
+        <v>0</v>
+      </c>
+      <c r="D51" s="11">
+        <v>0</v>
+      </c>
+      <c r="E51" s="11">
+        <v>0</v>
+      </c>
+      <c r="F51" s="11">
+        <v>0</v>
+      </c>
+      <c r="G51" s="11">
+        <v>0</v>
+      </c>
+      <c r="H51" s="11">
+        <v>0</v>
+      </c>
+      <c r="I51" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>